<commit_message>
abm alumnos con archivo ok
</commit_message>
<xml_diff>
--- a/division_tareas.xlsx
+++ b/division_tareas.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gui\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edalesio\Desktop\TP\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2820" yWindow="0" windowWidth="27720" windowHeight="12645"/>
+    <workbookView minimized="1" xWindow="2820" yWindow="0" windowWidth="27720" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$C$16</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -104,7 +104,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -154,7 +154,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -416,13 +416,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="43.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34" bestFit="1" customWidth="1"/>
@@ -463,7 +464,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -479,7 +480,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -487,7 +488,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -498,7 +499,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -517,7 +518,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -572,7 +573,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C1">
+  <autoFilter ref="A1:C16">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Emi"/>
+        <filter val="Juan"/>
+      </filters>
+    </filterColumn>
     <sortState ref="A2:C16">
       <sortCondition ref="C1"/>
     </sortState>

</xml_diff>